<commit_message>
Add support for text formula cells. Evaluate formula cell prior to date formatted check to prevent "Cannot get a numeric value from a text formula cell" exception.
</commit_message>
<xml_diff>
--- a/test/dk/ative/docjure/testdata/formulae.xlsx
+++ b/test/dk/ative/docjure/testdata/formulae.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,12 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Formula</t>
   </si>
   <si>
     <t>Expected value</t>
+  </si>
+  <si>
+    <t>String Formula</t>
   </si>
 </sst>
 </file>
@@ -37,6 +40,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -399,18 +403,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,7 +423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <f>1</f>
         <v>1</v>
@@ -427,7 +432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <f>2+2</f>
         <v>4</v>
@@ -436,7 +441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <f>2*3</f>
         <v>6</v>
@@ -445,7 +450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
         <f>DATE(2014,10,9)</f>
         <v>41921</v>
@@ -454,13 +459,22 @@
         <v>41921</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="1">
         <f>DATE(2010,10,27)+17</f>
         <v>40495</v>
       </c>
       <c r="B6" s="1">
         <v>40495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="str">
+        <f>"String"&amp;" "&amp;"Formula"</f>
+        <v>String Formula</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>